<commit_message>
- Made tracker.track_next_frame() return True rather than None when a frame has been read successfully. The last commit made it return False when a frame is not read successfully, and made the tracking loop in track.ipynb stop when that happens. However None was interpreted as False, which meant the tracking loop would never proceed.
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t xml:space="preserve">trial(s)</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">bkgSub_options.secondary_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pa_Fri_43dpf_GroupC_n5_20200711_1550</t>
   </si>
   <si>
     <t xml:space="preserve">Pa_Sun_7dpf_GroupB_n2a_20200614_1455</t>
@@ -102,7 +105,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,6 +139,11 @@
       <name val="FreeSans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -201,7 +209,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,6 +231,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,13 +318,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.11"/>
@@ -439,91 +451,103 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>1332</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1332</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>1332</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4" t="n">
-        <v>1370</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>1370</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>1370</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>1335</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1335</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1"/>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>1335</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
- tracker/utils.py: Added functions to load tracker settings files.
- viewer.py: Added a tab called "Tune" to visualize the effect of tuning detection parameters.
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t xml:space="preserve">trial(s)</t>
   </si>
@@ -44,6 +44,43 @@
   </si>
   <si>
     <t xml:space="preserve">*_84dpf_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pa_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[SR]?_*_7dpf_*</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[SR]?_*_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[4578]?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">dpf_*</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Pa_Fri_7dpf_GroupD_n2_20200605_1400</t>
@@ -218,6 +255,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,10 +272,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,13 +355,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.11"/>
@@ -387,167 +424,200 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="n">
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="n">
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="n">
         <v>1253</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="n">
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="n">
         <v>1253</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="C14" s="3" t="n">
+        <v>1332</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>1332</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="C16" s="5" t="n">
+        <v>1370</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>1332</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="C17" s="5" t="n">
+        <v>1370</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>1335</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>1332</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4" t="n">
-        <v>1370</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>1370</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="n">
+      <c r="C19" s="3" t="n">
         <v>1335</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>1335</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1"/>
+      <c r="D19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>